<commit_message>
Update Leave Card 6/8/2023 4:36 PM
</commit_message>
<xml_diff>
--- a/NEW HR/DONE/DORADO, JULIADA.xlsx
+++ b/NEW HR/DONE/DORADO, JULIADA.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\NEW HR\DONE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JHL336T\Users\ASUS\Desktop\LEAVE-CARD\NEW HR\DONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTION" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>PERIOD</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>4/20,28/2023</t>
+  </si>
+  <si>
+    <t>06/6,9,14,16,20,23,27,30/2023</t>
   </si>
 </sst>
 </file>
@@ -638,6 +641,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -650,20 +662,11 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1360,7 +1363,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B5D8F3C-4FD5-4318-83F6-163B56792B3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1403,7 +1406,7 @@
         <xdr:cNvPr id="5" name="TextBox 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0BAE224-67DC-A2F7-0A1F-28CB86DFB7CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1467,7 +1470,7 @@
         <xdr:cNvPr id="4" name="Arrow: Left 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7243AC54-FD55-C7CF-DEF3-E45E6F99CAA1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1530,7 @@
         <xdr:cNvPr id="8" name="Oval 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CEC4AD9-D5D6-0CFD-8D82-CC23F90E3707}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1593,7 +1596,7 @@
         <xdr:cNvPr id="9" name="Arrow: Left-Right 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAE8B24D-B9B9-4AB0-AE94-782594B55A03}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,7 +1659,7 @@
         <xdr:cNvPr id="10" name="TextBox 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D163C4F0-3D7F-3E52-4B17-0D29F1241915}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1754,7 +1757,7 @@
         <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{642CA079-93A1-34E3-CEF5-F7D33015D895}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1813,7 +1816,7 @@
         <xdr:cNvPr id="19" name="TextBox 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{784FECEA-1780-3E7F-7EBB-9F8254797C91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1878,7 +1881,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCCE859-255F-F039-E92D-1510F02C6167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1921,7 +1924,7 @@
         <xdr:cNvPr id="21" name="TextBox 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A7AA7C6-9540-EB37-E3D2-9A2A68BD6824}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1996,7 +1999,7 @@
         <xdr:cNvPr id="22" name="TextBox 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1674299-9801-A253-3871-18715F4FF740}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2182,7 +2185,7 @@
         <xdr:cNvPr id="23" name="Oval 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66C92862-99CA-461F-932E-30DFD0874402}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2248,7 +2251,7 @@
         <xdr:cNvPr id="24" name="Straight Arrow Connector 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD20A152-8288-4C69-BE76-AD8E41A960CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2306,7 +2309,7 @@
         <xdr:cNvPr id="26" name="Oval 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE7E56BE-0B3E-4110-A5A9-44C888A46B90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2372,7 +2375,7 @@
         <xdr:cNvPr id="27" name="Straight Arrow Connector 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C33E41C1-1592-4272-A561-4833666913C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2428,7 +2431,7 @@
         <xdr:cNvPr id="30" name="TextBox 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C655B57-0D66-4740-B73E-75D1E106F99A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2503,7 +2506,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0284C105-1E11-4529-B509-D655B8C5279A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2546,7 +2549,7 @@
         <xdr:cNvPr id="32" name="Oval 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E73E9A40-2B3C-47DC-9C07-7C65795CE0A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2612,7 +2615,7 @@
         <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32002197-8137-42BA-B3E7-2690738DB64B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2668,7 +2671,7 @@
         <xdr:cNvPr id="34" name="TextBox 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A781E01A-37B6-4259-9759-556FE6893D51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2766,7 +2769,7 @@
         <xdr:cNvPr id="2" name="Rectangle 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C99D8E5F-2D60-FF91-2593-A29CC276458B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2829,7 +2832,7 @@
         <xdr:cNvPr id="3" name="Rectangle 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E6A331-FC2C-4EF9-8F5B-65908D453D1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3305,10 +3308,10 @@
   </sheetPr>
   <dimension ref="A2:K134"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="4050" topLeftCell="A70" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="4050" topLeftCell="A73" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+      <selection pane="bottomLeft" activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,14 +3341,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -3356,16 +3359,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="58">
         <v>38311</v>
       </c>
-      <c r="G3" s="56"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -3378,14 +3381,14 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="59"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -3411,18 +3414,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -3469,7 +3472,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table15[EARNED])-SUM(Table15[Absence Undertime W/ Pay])</f>
-        <v>53.75</v>
+        <v>56.25</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -3479,7 +3482,7 @@
       <c r="H9" s="11"/>
       <c r="I9" s="13">
         <f>SUM(Table15[[EARNED ]])-SUM(Table15[Absence Undertime  W/ Pay])</f>
-        <v>76.75</v>
+        <v>79.25</v>
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
@@ -4887,13 +4890,15 @@
       <c r="B79" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C79" s="13"/>
+      <c r="C79" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D79" s="39"/>
       <c r="E79" s="9"/>
       <c r="F79" s="20"/>
-      <c r="G79" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G79" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H79" s="39">
         <v>2</v>
@@ -4905,15 +4910,19 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" s="40"/>
+      <c r="A80" s="40">
+        <v>45047</v>
+      </c>
       <c r="B80" s="20"/>
-      <c r="C80" s="13"/>
+      <c r="C80" s="13">
+        <v>1.25</v>
+      </c>
       <c r="D80" s="39"/>
       <c r="E80" s="9"/>
       <c r="F80" s="20"/>
-      <c r="G80" s="13" t="str">
-        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
-        <v/>
+      <c r="G80" s="13">
+        <f>IF(ISBLANK(Table15[[#This Row],[EARNED]]),"",Table15[[#This Row],[EARNED]])</f>
+        <v>1.25</v>
       </c>
       <c r="H80" s="39"/>
       <c r="I80" s="9"/>
@@ -4921,7 +4930,9 @@
       <c r="K80" s="20"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="40"/>
+      <c r="A81" s="40">
+        <v>45078</v>
+      </c>
       <c r="B81" s="20"/>
       <c r="C81" s="13"/>
       <c r="D81" s="39"/>
@@ -5786,17 +5797,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
@@ -5831,10 +5842,10 @@
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
       <pane ySplit="3690" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="E9" sqref="E9"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,14 +5876,14 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="54"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
@@ -5886,17 +5897,17 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="55">
+      <c r="F3" s="58">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F3:G3),"---------",'2018 LEAVE CREDITS'!F3:G3)</f>
         <v>38311</v>
       </c>
-      <c r="G3" s="56"/>
+      <c r="G3" s="52"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="58"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="60"/>
     </row>
     <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
@@ -5910,17 +5921,17 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="56" t="str">
+      <c r="F4" s="52" t="str">
         <f>IF(ISBLANK('2018 LEAVE CREDITS'!F4:G4),"",'2018 LEAVE CREDITS'!F4:G4)</f>
         <v/>
       </c>
-      <c r="G4" s="56"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="59"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="53"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -5946,18 +5957,18 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60" t="s">
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
       <c r="K7" s="14"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -6004,7 +6015,7 @@
       <c r="D9" s="11"/>
       <c r="E9" s="13">
         <f>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</f>
-        <v>63.986999999999995</v>
+        <v>55.986999999999995</v>
       </c>
       <c r="F9" s="11"/>
       <c r="G9" s="13" t="str">
@@ -6286,10 +6297,16 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="40">
+        <v>45078</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>65</v>
+      </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="39">
+        <v>8</v>
+      </c>
       <c r="E22" s="9"/>
       <c r="F22" s="20"/>
       <c r="G22" s="13" t="str">
@@ -6299,7 +6316,9 @@
       <c r="H22" s="39"/>
       <c r="I22" s="9"/>
       <c r="J22" s="11"/>
-      <c r="K22" s="20"/>
+      <c r="K22" s="20" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>

</xml_diff>